<commit_message>
Updates to GBSC, BPEiC, PERAC, and newest MDL version from US model
</commit_message>
<xml_diff>
--- a/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
+++ b/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
@@ -1,27 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\elec\GBSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\RMI\Minnesota\MN_Model\InputData\elec\GBSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A638F84-8FA8-49E7-8310-4C7EBB4F24E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DEAAF6-2DD6-4E5A-B79D-733CE31E7D8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="60" windowWidth="21615" windowHeight="16485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1350" yWindow="855" windowWidth="12375" windowHeight="15510" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="AEO Table 9" sheetId="4" r:id="rId2"/>
     <sheet name="AEO Table 9 (2019)" sheetId="8" r:id="rId3"/>
     <sheet name="RE Futures Data &amp; Calcs" sheetId="6" r:id="rId4"/>
-    <sheet name="BGBSC" sheetId="3" r:id="rId5"/>
-    <sheet name="PAGBSC" sheetId="5" r:id="rId6"/>
-    <sheet name="SYGBSC" sheetId="9" r:id="rId7"/>
+    <sheet name="Potential" sheetId="10" r:id="rId5"/>
+    <sheet name="BGBSC" sheetId="3" r:id="rId6"/>
+    <sheet name="PAGBSC" sheetId="5" r:id="rId7"/>
+    <sheet name="SYGBSC" sheetId="9" r:id="rId8"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId9"/>
+  </externalReferences>
   <definedNames>
+    <definedName name="gigwatts_to_megawatts" localSheetId="4">[1]About!$A$35</definedName>
     <definedName name="gigwatts_to_megawatts">About!$A$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -61,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="181">
   <si>
     <t>Source:</t>
   </si>
@@ -601,6 +606,9 @@
   </si>
   <si>
     <t>GBSC Start Year Grid Battery Storage Capacity</t>
+  </si>
+  <si>
+    <t>Policy scenario</t>
   </si>
 </sst>
 </file>
@@ -1257,6 +1265,35 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="About"/>
+      <sheetName val="AEO Table 9"/>
+      <sheetName val="AEO Table 9 (2019)"/>
+      <sheetName val="BGBSC"/>
+      <sheetName val="PAGBSC"/>
+      <sheetName val="SYGBSC"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="35">
+          <cell r="A35">
+            <v>1000</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1580,7 +1617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16539,6 +16576,198 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E7F44C-4F44-443E-B514-8EF24C7D8CB6}">
+  <dimension ref="A1:AG20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" style="6" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="6">
+        <v>2019</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="6">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+    </row>
+    <row r="17" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="7"/>
+      <c r="AE17" s="7"/>
+      <c r="AF17" s="7"/>
+      <c r="AG17" s="7"/>
+    </row>
+    <row r="18" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="28"/>
+      <c r="U18" s="28"/>
+      <c r="V18" s="28"/>
+      <c r="W18" s="28"/>
+      <c r="X18" s="28"/>
+      <c r="Y18" s="28"/>
+      <c r="Z18" s="28"/>
+      <c r="AA18" s="28"/>
+      <c r="AB18" s="28"/>
+      <c r="AC18" s="28"/>
+      <c r="AD18" s="28"/>
+      <c r="AE18" s="28"/>
+      <c r="AF18" s="28"/>
+      <c r="AG18" s="28"/>
+    </row>
+    <row r="19" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="28"/>
+      <c r="S19" s="28"/>
+      <c r="T19" s="28"/>
+      <c r="U19" s="28"/>
+      <c r="V19" s="28"/>
+      <c r="W19" s="28"/>
+      <c r="X19" s="28"/>
+      <c r="Y19" s="28"/>
+      <c r="Z19" s="28"/>
+      <c r="AA19" s="28"/>
+      <c r="AB19" s="28"/>
+      <c r="AC19" s="28"/>
+      <c r="AD19" s="28"/>
+      <c r="AE19" s="28"/>
+      <c r="AF19" s="28"/>
+      <c r="AG19" s="28"/>
+    </row>
+    <row r="20" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="28"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="28"/>
+      <c r="U20" s="28"/>
+      <c r="V20" s="28"/>
+      <c r="W20" s="28"/>
+      <c r="X20" s="28"/>
+      <c r="Y20" s="28"/>
+      <c r="Z20" s="28"/>
+      <c r="AA20" s="28"/>
+      <c r="AB20" s="28"/>
+      <c r="AC20" s="28"/>
+      <c r="AD20" s="28"/>
+      <c r="AE20" s="28"/>
+      <c r="AF20" s="28"/>
+      <c r="AG20" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -16793,14 +17022,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E930CD6-BDBE-4B51-AE85-855FFBE243D6}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AG14" sqref="AG14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16915,132 +17146,132 @@
         <v>140</v>
       </c>
       <c r="B2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!B20*gigwatts_to_megawatts</f>
-        <v>-6.141753772226366E-10</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!B1)</f>
+        <v>1000</v>
       </c>
       <c r="C2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!C20*gigwatts_to_megawatts</f>
-        <v>2568.1077419347134</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!C1)</f>
+        <v>4193.5483870971948</v>
       </c>
       <c r="D2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!D20*gigwatts_to_megawatts</f>
-        <v>3394.8754838700406</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!D1)</f>
+        <v>7387.0967741934583</v>
       </c>
       <c r="E2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!E20*gigwatts_to_megawatts</f>
-        <v>6590.6432258062787</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!E1)</f>
+        <v>10580.645161290653</v>
       </c>
       <c r="F2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!F20*gigwatts_to_megawatts</f>
-        <v>9786.4099677416052</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!F1)</f>
+        <v>13774.193548386917</v>
       </c>
       <c r="G2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!G20*gigwatts_to_megawatts</f>
-        <v>12983.177709676933</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!G1)</f>
+        <v>16967.741935484111</v>
       </c>
       <c r="H2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!H20*gigwatts_to_megawatts</f>
-        <v>16366.945451612261</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!H1)</f>
+        <v>20161.290322580375</v>
       </c>
       <c r="I2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!I20*gigwatts_to_megawatts</f>
-        <v>19782.713193547588</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!I1)</f>
+        <v>23354.83870967757</v>
       </c>
       <c r="J2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!J20*gigwatts_to_megawatts</f>
-        <v>23198.480935482916</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!J1)</f>
+        <v>26548.387096773833</v>
       </c>
       <c r="K2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!K20*gigwatts_to_megawatts</f>
-        <v>26614.248677419157</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!K1)</f>
+        <v>29741.935483871028</v>
       </c>
       <c r="L2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!L20*gigwatts_to_megawatts</f>
-        <v>29979.035419354481</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!L1)</f>
+        <v>32935.483870968223</v>
       </c>
       <c r="M2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!M20*gigwatts_to_megawatts</f>
-        <v>33394.803161289805</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!M1)</f>
+        <v>36129.032258064486</v>
       </c>
       <c r="N2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!N20*gigwatts_to_megawatts</f>
-        <v>37221.570903225132</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!N1)</f>
+        <v>39322.580645161681</v>
       </c>
       <c r="O2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!O20*gigwatts_to_megawatts</f>
-        <v>41048.33864516046</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!O1)</f>
+        <v>42516.129032257944</v>
       </c>
       <c r="P2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!P20*gigwatts_to_megawatts</f>
-        <v>44588.082387095797</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!P1)</f>
+        <v>45709.677419355139</v>
       </c>
       <c r="Q2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!Q20*gigwatts_to_megawatts</f>
-        <v>47967.168129032034</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!Q1)</f>
+        <v>48903.225806451403</v>
       </c>
       <c r="R2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!R20*gigwatts_to_megawatts</f>
-        <v>51793.935870967362</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!R1)</f>
+        <v>52096.774193548597</v>
       </c>
       <c r="S2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!S20*gigwatts_to_megawatts</f>
-        <v>55553.119612902687</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!S1)</f>
+        <v>55290.322580644861</v>
       </c>
       <c r="T2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!T20*gigwatts_to_megawatts</f>
-        <v>59379.887354838014</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!T1)</f>
+        <v>58483.870967742056</v>
       </c>
       <c r="U2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!U20*gigwatts_to_megawatts</f>
-        <v>63191.855096773339</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!U1)</f>
+        <v>61677.41935483925</v>
       </c>
       <c r="V2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!V20*gigwatts_to_megawatts</f>
-        <v>67018.622838708659</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!V1)</f>
+        <v>64870.967741935514</v>
       </c>
       <c r="W2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!W20*gigwatts_to_megawatts</f>
-        <v>70758.041580644902</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!W1)</f>
+        <v>68064.516129032709</v>
       </c>
       <c r="X2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!X20*gigwatts_to_megawatts</f>
-        <v>74145.410322580239</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!X1)</f>
+        <v>71258.064516128972</v>
       </c>
       <c r="Y2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!Y20*gigwatts_to_megawatts</f>
-        <v>77377.454064515565</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!Y1)</f>
+        <v>74451.612903226167</v>
       </c>
       <c r="Z2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!Z20*gigwatts_to_megawatts</f>
-        <v>81204.221806450892</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!Z1)</f>
+        <v>77645.16129032243</v>
       </c>
       <c r="AA2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!AA20*gigwatts_to_megawatts</f>
-        <v>85030.98954838622</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!AA1)</f>
+        <v>80838.709677419625</v>
       </c>
       <c r="AB2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!AB20*gigwatts_to_megawatts</f>
-        <v>88223.900290321544</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!AB1)</f>
+        <v>84032.258064515889</v>
       </c>
       <c r="AC2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!AC20*gigwatts_to_megawatts</f>
-        <v>91371.272032257781</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!AC1)</f>
+        <v>87225.806451613083</v>
       </c>
       <c r="AD2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!AD20*gigwatts_to_megawatts</f>
-        <v>93438.02377419312</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!AD1)</f>
+        <v>90419.354838709347</v>
       </c>
       <c r="AE2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!AE20*gigwatts_to_megawatts</f>
-        <v>96263.782516128427</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!AE1)</f>
+        <v>93612.903225806542</v>
       </c>
       <c r="AF2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!AF20*gigwatts_to_megawatts</f>
-        <v>98807.126258063756</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!AF1)</f>
+        <v>96806.451612903737</v>
       </c>
       <c r="AG2" s="8">
-        <f>'RE Futures Data &amp; Calcs'!AG20*gigwatts_to_megawatts</f>
-        <v>102599.10399999909</v>
+        <f>TREND(Potential!$B$3:$C$3,Potential!$B$2:$C$2,PAGBSC!AG1)</f>
+        <v>100000</v>
       </c>
     </row>
   </sheetData>
@@ -17049,7 +17280,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59172300-46A9-4F58-8C21-81ABD9E9BA2D}">
   <sheetPr>
     <tabColor theme="3"/>

</xml_diff>